<commit_message>
changed affinity of Shapaja occurrences to Tropical
For some reason, didn't work with the loop
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/EarlyMidLate_epochs.xlsx
+++ b/data_2023/time_bins/EarlyMidLate_epochs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">interval_name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">color</t>
   </si>
   <si>
+    <t xml:space="preserve">abbr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Late Holocene</t>
   </si>
   <si>
@@ -73,12 +76,18 @@
     <t xml:space="preserve">#FEE6AA</t>
   </si>
   <si>
+    <t xml:space="preserve">Late</t>
+  </si>
+  <si>
     <t xml:space="preserve">Early Oligocene</t>
   </si>
   <si>
     <t xml:space="preserve">#FED99A</t>
   </si>
   <si>
+    <t xml:space="preserve">Early</t>
+  </si>
+  <si>
     <t xml:space="preserve">Late Eocene</t>
   </si>
   <si>
@@ -89,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">#FCB482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid</t>
   </si>
   <si>
     <t xml:space="preserve">Early Eocene</t>
@@ -304,13 +316,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.55"/>
   </cols>
@@ -328,10 +340,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -342,7 +357,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0.0042</v>
@@ -353,7 +368,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0.0082</v>
@@ -364,7 +379,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>0.0117</v>
@@ -375,7 +390,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>0.129</v>
@@ -386,7 +401,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0.774</v>
@@ -397,7 +412,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>2.58</v>
@@ -408,7 +423,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>3.6</v>
@@ -419,7 +434,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>5.333</v>
@@ -430,7 +445,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>11.63</v>
@@ -441,7 +456,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>15.97</v>
@@ -452,7 +467,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>23.03</v>
@@ -461,12 +476,15 @@
         <v>27.82</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>27.82</v>
@@ -475,12 +493,15 @@
         <v>33.9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>33.9</v>
@@ -489,12 +510,15 @@
         <v>37.71</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>37.71</v>
@@ -503,12 +527,15 @@
         <v>47.8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>47.8</v>
@@ -517,12 +544,15 @@
         <v>56</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>56</v>
@@ -533,7 +563,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>59.2</v>
@@ -544,7 +574,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>61.6</v>

</xml_diff>

<commit_message>
changing Mustersan in SALMA_smoothed
</commit_message>
<xml_diff>
--- a/data_2023/time_bins/EarlyMidLate_epochs.xlsx
+++ b/data_2023/time_bins/EarlyMidLate_epochs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t xml:space="preserve">interval_name</t>
   </si>
@@ -67,9 +67,18 @@
     <t xml:space="preserve">Middle Miocene</t>
   </si>
   <si>
+    <t xml:space="preserve">#FFFF4D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Early Miocene</t>
   </si>
   <si>
+    <t xml:space="preserve">#FFFF33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Early</t>
+  </si>
+  <si>
     <t xml:space="preserve">Late Oligocene</t>
   </si>
   <si>
@@ -85,9 +94,6 @@
     <t xml:space="preserve">#FED99A</t>
   </si>
   <si>
-    <t xml:space="preserve">Early</t>
-  </si>
-  <si>
     <t xml:space="preserve">Late Eocene</t>
   </si>
   <si>
@@ -112,7 +118,13 @@
     <t xml:space="preserve">Late Paleocene</t>
   </si>
   <si>
+    <t xml:space="preserve">#FDBF6F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Middle Paleocene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#FEBF65</t>
   </si>
   <si>
     <t xml:space="preserve">Early Paleocene</t>
@@ -319,7 +331,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,10 +465,13 @@
       <c r="C11" s="3" t="n">
         <v>15.97</v>
       </c>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>15.97</v>
@@ -464,10 +479,16 @@
       <c r="C12" s="3" t="n">
         <v>23.03</v>
       </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>23.03</v>
@@ -476,15 +497,15 @@
         <v>27.82</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="n">
         <v>27.82</v>
@@ -493,15 +514,15 @@
         <v>33.9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="n">
         <v>33.9</v>
@@ -510,15 +531,15 @@
         <v>37.71</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="n">
         <v>37.71</v>
@@ -527,15 +548,15 @@
         <v>47.8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>47.8</v>
@@ -544,15 +565,15 @@
         <v>56</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="n">
         <v>56</v>
@@ -560,10 +581,13 @@
       <c r="C18" s="3" t="n">
         <v>59.2</v>
       </c>
+      <c r="D18" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3" t="n">
         <v>59.2</v>
@@ -571,10 +595,13 @@
       <c r="C19" s="3" t="n">
         <v>61.6</v>
       </c>
+      <c r="D19" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3" t="n">
         <v>61.6</v>

</xml_diff>